<commit_message>
Insert lines about recently decision of interest rate
</commit_message>
<xml_diff>
--- a/interestRate.xlsx
+++ b/interestRate.xlsx
@@ -13,14 +13,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$D$210</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$F$81</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$F$85</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="64">
   <si>
     <t>UP</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -321,7 +321,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -347,6 +347,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -644,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F213"/>
+  <dimension ref="A1:F217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="J76" sqref="J76"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
@@ -679,9 +682,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1">
-      <c r="A2" s="6">
-        <v>42613</v>
+    <row r="2" spans="1:6" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A2" s="9">
+        <v>42735</v>
       </c>
       <c r="B2" s="7">
         <v>1.25</v>
@@ -700,9 +703,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1">
-      <c r="A3" s="6">
-        <v>42582</v>
+    <row r="3" spans="1:6" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A3" s="9">
+        <v>42704</v>
       </c>
       <c r="B3" s="7">
         <v>1.25</v>
@@ -721,16 +724,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1">
-      <c r="A4" s="6">
-        <v>42551</v>
+    <row r="4" spans="1:6" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A4" s="9">
+        <v>42674</v>
       </c>
       <c r="B4" s="7">
         <v>1.25</v>
       </c>
       <c r="C4" s="7" t="str">
-        <f t="shared" ref="C4:C65" si="0">IF(B4-B5=0,"STAY",IF(B4&gt;B5,"UP","DOWN"))</f>
-        <v>DOWN</v>
+        <f>IF(B4-B5=0,"STAY",IF(B4&gt;B5,"UP","DOWN"))</f>
+        <v>STAY</v>
       </c>
       <c r="D4" s="7">
         <v>6</v>
@@ -742,15 +745,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1">
-      <c r="A5" s="6">
-        <v>42521</v>
+    <row r="5" spans="1:6" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="A5" s="9">
+        <v>42643</v>
       </c>
       <c r="B5" s="7">
-        <v>1.5</v>
+        <v>1.25</v>
       </c>
       <c r="C5" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B5-B6=0,"STAY",IF(B5&gt;B6,"UP","DOWN"))</f>
         <v>STAY</v>
       </c>
       <c r="D5" s="7">
@@ -765,70 +768,70 @@
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1">
       <c r="A6" s="6">
-        <v>42490</v>
+        <v>42613</v>
       </c>
       <c r="B6" s="7">
-        <v>1.5</v>
+        <v>1.25</v>
       </c>
       <c r="C6" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B6-B7=0,"STAY",IF(B6&gt;B7,"UP","DOWN"))</f>
         <v>STAY</v>
       </c>
       <c r="D6" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E6" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1">
       <c r="A7" s="6">
-        <v>42460</v>
+        <v>42582</v>
       </c>
       <c r="B7" s="7">
-        <v>1.5</v>
+        <v>1.25</v>
       </c>
       <c r="C7" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(B7-B8=0,"STAY",IF(B7&gt;B8,"UP","DOWN"))</f>
         <v>STAY</v>
       </c>
       <c r="D7" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E7" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1">
       <c r="A8" s="6">
-        <v>42429</v>
+        <v>42551</v>
       </c>
       <c r="B8" s="7">
-        <v>1.5</v>
+        <v>1.25</v>
       </c>
       <c r="C8" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>STAY</v>
+        <f t="shared" ref="C8:C69" si="0">IF(B8-B9=0,"STAY",IF(B8&gt;B9,"UP","DOWN"))</f>
+        <v>DOWN</v>
       </c>
       <c r="D8" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E8" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1">
       <c r="A9" s="6">
-        <v>42400</v>
+        <v>42521</v>
       </c>
       <c r="B9" s="7">
         <v>1.5</v>
@@ -849,7 +852,7 @@
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1">
       <c r="A10" s="6">
-        <v>42369</v>
+        <v>42490</v>
       </c>
       <c r="B10" s="7">
         <v>1.5</v>
@@ -859,18 +862,18 @@
         <v>STAY</v>
       </c>
       <c r="D10" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E10" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1">
       <c r="A11" s="6">
-        <v>42338</v>
+        <v>42460</v>
       </c>
       <c r="B11" s="7">
         <v>1.5</v>
@@ -880,18 +883,18 @@
         <v>STAY</v>
       </c>
       <c r="D11" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E11" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1">
       <c r="A12" s="6">
-        <v>42308</v>
+        <v>42429</v>
       </c>
       <c r="B12" s="7">
         <v>1.5</v>
@@ -901,18 +904,18 @@
         <v>STAY</v>
       </c>
       <c r="D12" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E12" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1">
       <c r="A13" s="6">
-        <v>42277</v>
+        <v>42400</v>
       </c>
       <c r="B13" s="7">
         <v>1.5</v>
@@ -933,7 +936,7 @@
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1">
       <c r="A14" s="6">
-        <v>42247</v>
+        <v>42369</v>
       </c>
       <c r="B14" s="7">
         <v>1.5</v>
@@ -954,7 +957,7 @@
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1">
       <c r="A15" s="6">
-        <v>42216</v>
+        <v>42338</v>
       </c>
       <c r="B15" s="7">
         <v>1.5</v>
@@ -975,322 +978,322 @@
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1">
       <c r="A16" s="6">
-        <v>42185</v>
+        <v>42308</v>
       </c>
       <c r="B16" s="7">
         <v>1.5</v>
       </c>
       <c r="C16" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>DOWN</v>
+        <v>STAY</v>
       </c>
       <c r="D16" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E16" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1">
       <c r="A17" s="6">
-        <v>42155</v>
+        <v>42277</v>
       </c>
       <c r="B17" s="7">
-        <v>1.75</v>
+        <v>1.5</v>
       </c>
       <c r="C17" s="7" t="str">
         <f t="shared" si="0"/>
         <v>STAY</v>
       </c>
       <c r="D17" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E17" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1">
       <c r="A18" s="6">
-        <v>42124</v>
+        <v>42247</v>
       </c>
       <c r="B18" s="7">
-        <v>1.75</v>
+        <v>1.5</v>
       </c>
       <c r="C18" s="7" t="str">
         <f t="shared" si="0"/>
         <v>STAY</v>
       </c>
       <c r="D18" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E18" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1">
       <c r="A19" s="6">
-        <v>42094</v>
+        <v>42216</v>
       </c>
       <c r="B19" s="7">
-        <v>1.75</v>
+        <v>1.5</v>
       </c>
       <c r="C19" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>DOWN</v>
+        <v>STAY</v>
       </c>
       <c r="D19" s="7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E19" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1">
       <c r="A20" s="6">
-        <v>42063</v>
+        <v>42185</v>
       </c>
       <c r="B20" s="7">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="C20" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>STAY</v>
+        <v>DOWN</v>
       </c>
       <c r="D20" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E20" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1">
       <c r="A21" s="6">
-        <v>42035</v>
+        <v>42155</v>
       </c>
       <c r="B21" s="7">
-        <v>2</v>
+        <v>1.75</v>
       </c>
       <c r="C21" s="7" t="str">
         <f t="shared" si="0"/>
         <v>STAY</v>
       </c>
       <c r="D21" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E21" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1">
       <c r="A22" s="6">
-        <v>42004</v>
+        <v>42124</v>
       </c>
       <c r="B22" s="7">
-        <v>2</v>
+        <v>1.75</v>
       </c>
       <c r="C22" s="7" t="str">
         <f t="shared" si="0"/>
         <v>STAY</v>
       </c>
       <c r="D22" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E22" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15" customHeight="1">
       <c r="A23" s="6">
-        <v>41973</v>
+        <v>42094</v>
       </c>
       <c r="B23" s="7">
+        <v>1.75</v>
+      </c>
+      <c r="C23" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>DOWN</v>
+      </c>
+      <c r="D23" s="7">
+        <v>4</v>
+      </c>
+      <c r="E23" s="7">
         <v>2</v>
       </c>
-      <c r="C23" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>STAY</v>
-      </c>
-      <c r="D23" s="7">
-        <v>6</v>
-      </c>
-      <c r="E23" s="7">
-        <v>0</v>
-      </c>
       <c r="F23" s="7" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15" customHeight="1">
       <c r="A24" s="6">
-        <v>41943</v>
+        <v>42063</v>
       </c>
       <c r="B24" s="7">
         <v>2</v>
       </c>
       <c r="C24" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>DOWN</v>
+        <v>STAY</v>
       </c>
       <c r="D24" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E24" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15" customHeight="1">
       <c r="A25" s="6">
-        <v>41912</v>
+        <v>42035</v>
       </c>
       <c r="B25" s="7">
-        <v>2.25</v>
+        <v>2</v>
       </c>
       <c r="C25" s="7" t="str">
         <f t="shared" si="0"/>
         <v>STAY</v>
       </c>
       <c r="D25" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E25" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15" customHeight="1">
       <c r="A26" s="6">
-        <v>41882</v>
+        <v>42004</v>
       </c>
       <c r="B26" s="7">
-        <v>2.25</v>
+        <v>2</v>
       </c>
       <c r="C26" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>DOWN</v>
+        <v>STAY</v>
       </c>
       <c r="D26" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E26" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15" customHeight="1">
       <c r="A27" s="6">
-        <v>41851</v>
+        <v>41973</v>
       </c>
       <c r="B27" s="7">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="C27" s="7" t="str">
         <f t="shared" si="0"/>
         <v>STAY</v>
       </c>
       <c r="D27" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E27" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1">
       <c r="A28" s="6">
-        <v>41820</v>
+        <v>41943</v>
       </c>
       <c r="B28" s="7">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="C28" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>STAY</v>
+        <v>DOWN</v>
       </c>
       <c r="D28" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E28" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1">
       <c r="A29" s="6">
-        <v>41790</v>
+        <v>41912</v>
       </c>
       <c r="B29" s="7">
-        <v>2.5</v>
+        <v>2.25</v>
       </c>
       <c r="C29" s="7" t="str">
         <f t="shared" si="0"/>
         <v>STAY</v>
       </c>
       <c r="D29" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E29" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1">
       <c r="A30" s="6">
-        <v>41759</v>
+        <v>41882</v>
       </c>
       <c r="B30" s="7">
-        <v>2.5</v>
+        <v>2.25</v>
       </c>
       <c r="C30" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>STAY</v>
+        <v>DOWN</v>
       </c>
       <c r="D30" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E30" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15" customHeight="1">
       <c r="A31" s="6">
-        <v>41729</v>
+        <v>41851</v>
       </c>
       <c r="B31" s="7">
         <v>2.5</v>
@@ -1300,18 +1303,18 @@
         <v>STAY</v>
       </c>
       <c r="D31" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E31" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15" customHeight="1">
       <c r="A32" s="6">
-        <v>41698</v>
+        <v>41820</v>
       </c>
       <c r="B32" s="7">
         <v>2.5</v>
@@ -1332,7 +1335,7 @@
     </row>
     <row r="33" spans="1:6" ht="15" customHeight="1">
       <c r="A33" s="6">
-        <v>41670</v>
+        <v>41790</v>
       </c>
       <c r="B33" s="7">
         <v>2.5</v>
@@ -1353,7 +1356,7 @@
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1">
       <c r="A34" s="6">
-        <v>41639</v>
+        <v>41759</v>
       </c>
       <c r="B34" s="7">
         <v>2.5</v>
@@ -1374,7 +1377,7 @@
     </row>
     <row r="35" spans="1:6" ht="15" customHeight="1">
       <c r="A35" s="6">
-        <v>41608</v>
+        <v>41729</v>
       </c>
       <c r="B35" s="7">
         <v>2.5</v>
@@ -1395,7 +1398,7 @@
     </row>
     <row r="36" spans="1:6" ht="15" customHeight="1">
       <c r="A36" s="6">
-        <v>41578</v>
+        <v>41698</v>
       </c>
       <c r="B36" s="7">
         <v>2.5</v>
@@ -1416,7 +1419,7 @@
     </row>
     <row r="37" spans="1:6" ht="15" customHeight="1">
       <c r="A37" s="6">
-        <v>41547</v>
+        <v>41670</v>
       </c>
       <c r="B37" s="7">
         <v>2.5</v>
@@ -1437,7 +1440,7 @@
     </row>
     <row r="38" spans="1:6" ht="15" customHeight="1">
       <c r="A38" s="6">
-        <v>41517</v>
+        <v>41639</v>
       </c>
       <c r="B38" s="7">
         <v>2.5</v>
@@ -1458,7 +1461,7 @@
     </row>
     <row r="39" spans="1:6" ht="15" customHeight="1">
       <c r="A39" s="6">
-        <v>41486</v>
+        <v>41608</v>
       </c>
       <c r="B39" s="7">
         <v>2.5</v>
@@ -1479,7 +1482,7 @@
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1">
       <c r="A40" s="6">
-        <v>41455</v>
+        <v>41578</v>
       </c>
       <c r="B40" s="7">
         <v>2.5</v>
@@ -1500,98 +1503,98 @@
     </row>
     <row r="41" spans="1:6" ht="15" customHeight="1">
       <c r="A41" s="6">
-        <v>41425</v>
+        <v>41547</v>
       </c>
       <c r="B41" s="7">
         <v>2.5</v>
       </c>
       <c r="C41" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>DOWN</v>
+        <v>STAY</v>
       </c>
       <c r="D41" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E41" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="15" customHeight="1">
       <c r="A42" s="6">
-        <v>41394</v>
+        <v>41517</v>
       </c>
       <c r="B42" s="7">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="C42" s="7" t="str">
         <f t="shared" si="0"/>
         <v>STAY</v>
       </c>
       <c r="D42" s="7">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E42" s="7">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="15" customHeight="1">
       <c r="A43" s="6">
-        <v>41364</v>
+        <v>41486</v>
       </c>
       <c r="B43" s="7">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="C43" s="7" t="str">
         <f t="shared" si="0"/>
         <v>STAY</v>
       </c>
       <c r="D43" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E43" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="15" customHeight="1">
       <c r="A44" s="6">
-        <v>41333</v>
+        <v>41455</v>
       </c>
       <c r="B44" s="7">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="C44" s="7" t="str">
         <f t="shared" si="0"/>
         <v>STAY</v>
       </c>
       <c r="D44" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E44" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="15" customHeight="1">
       <c r="A45" s="6">
-        <v>41305</v>
+        <v>41425</v>
       </c>
       <c r="B45" s="7">
-        <v>2.75</v>
+        <v>2.5</v>
       </c>
       <c r="C45" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>STAY</v>
+        <v>DOWN</v>
       </c>
       <c r="D45" s="7">
         <v>5</v>
@@ -1600,12 +1603,12 @@
         <v>1</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="15" customHeight="1">
       <c r="A46" s="6">
-        <v>41274</v>
+        <v>41394</v>
       </c>
       <c r="B46" s="7">
         <v>2.75</v>
@@ -1615,18 +1618,18 @@
         <v>STAY</v>
       </c>
       <c r="D46" s="7">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E46" s="7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="15" customHeight="1">
       <c r="A47" s="6">
-        <v>41243</v>
+        <v>41364</v>
       </c>
       <c r="B47" s="7">
         <v>2.75</v>
@@ -1636,63 +1639,63 @@
         <v>STAY</v>
       </c>
       <c r="D47" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E47" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="15" customHeight="1">
       <c r="A48" s="6">
-        <v>41213</v>
+        <v>41333</v>
       </c>
       <c r="B48" s="7">
         <v>2.75</v>
       </c>
       <c r="C48" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>DOWN</v>
+        <v>STAY</v>
       </c>
       <c r="D48" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E48" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="15" customHeight="1">
       <c r="A49" s="6">
-        <v>41182</v>
+        <v>41305</v>
       </c>
       <c r="B49" s="7">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="C49" s="7" t="str">
         <f t="shared" si="0"/>
         <v>STAY</v>
       </c>
       <c r="D49" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E49" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="15" customHeight="1">
       <c r="A50" s="6">
-        <v>41152</v>
+        <v>41274</v>
       </c>
       <c r="B50" s="7">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="C50" s="7" t="str">
         <f t="shared" si="0"/>
@@ -1710,35 +1713,35 @@
     </row>
     <row r="51" spans="1:6" ht="15" customHeight="1">
       <c r="A51" s="6">
-        <v>41121</v>
+        <v>41243</v>
       </c>
       <c r="B51" s="7">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="C51" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>DOWN</v>
+        <v>STAY</v>
       </c>
       <c r="D51" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E51" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="15" customHeight="1">
       <c r="A52" s="6">
-        <v>41090</v>
+        <v>41213</v>
       </c>
       <c r="B52" s="7">
-        <v>3.25</v>
+        <v>2.75</v>
       </c>
       <c r="C52" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>STAY</v>
+        <v>DOWN</v>
       </c>
       <c r="D52" s="7">
         <v>6</v>
@@ -1747,15 +1750,15 @@
         <v>0</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="15" customHeight="1">
       <c r="A53" s="6">
-        <v>41060</v>
+        <v>41182</v>
       </c>
       <c r="B53" s="7">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="C53" s="7" t="str">
         <f t="shared" si="0"/>
@@ -1773,10 +1776,10 @@
     </row>
     <row r="54" spans="1:6" ht="15" customHeight="1">
       <c r="A54" s="6">
-        <v>41029</v>
+        <v>41152</v>
       </c>
       <c r="B54" s="7">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="C54" s="7" t="str">
         <f t="shared" si="0"/>
@@ -1794,28 +1797,28 @@
     </row>
     <row r="55" spans="1:6" ht="15" customHeight="1">
       <c r="A55" s="6">
-        <v>40999</v>
+        <v>41121</v>
       </c>
       <c r="B55" s="7">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="C55" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>STAY</v>
+        <v>DOWN</v>
       </c>
       <c r="D55" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E55" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="15" customHeight="1">
       <c r="A56" s="6">
-        <v>40968</v>
+        <v>41090</v>
       </c>
       <c r="B56" s="7">
         <v>3.25</v>
@@ -1836,7 +1839,7 @@
     </row>
     <row r="57" spans="1:6" ht="15" customHeight="1">
       <c r="A57" s="6">
-        <v>40939</v>
+        <v>41060</v>
       </c>
       <c r="B57" s="7">
         <v>3.25</v>
@@ -1857,7 +1860,7 @@
     </row>
     <row r="58" spans="1:6" ht="15" customHeight="1">
       <c r="A58" s="6">
-        <v>40908</v>
+        <v>41029</v>
       </c>
       <c r="B58" s="7">
         <v>3.25</v>
@@ -1878,7 +1881,7 @@
     </row>
     <row r="59" spans="1:6" ht="15" customHeight="1">
       <c r="A59" s="6">
-        <v>40877</v>
+        <v>40999</v>
       </c>
       <c r="B59" s="7">
         <v>3.25</v>
@@ -1899,7 +1902,7 @@
     </row>
     <row r="60" spans="1:6" ht="15" customHeight="1">
       <c r="A60" s="6">
-        <v>40847</v>
+        <v>40968</v>
       </c>
       <c r="B60" s="7">
         <v>3.25</v>
@@ -1920,7 +1923,7 @@
     </row>
     <row r="61" spans="1:6" ht="15" customHeight="1">
       <c r="A61" s="6">
-        <v>40816</v>
+        <v>40939</v>
       </c>
       <c r="B61" s="7">
         <v>3.25</v>
@@ -1930,18 +1933,18 @@
         <v>STAY</v>
       </c>
       <c r="D61" s="7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E61" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F61" s="7" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="15" customHeight="1">
       <c r="A62" s="6">
-        <v>40786</v>
+        <v>40908</v>
       </c>
       <c r="B62" s="7">
         <v>3.25</v>
@@ -1962,7 +1965,7 @@
     </row>
     <row r="63" spans="1:6" ht="15" customHeight="1">
       <c r="A63" s="6">
-        <v>40755</v>
+        <v>40877</v>
       </c>
       <c r="B63" s="7">
         <v>3.25</v>
@@ -1983,14 +1986,14 @@
     </row>
     <row r="64" spans="1:6" ht="15" customHeight="1">
       <c r="A64" s="6">
-        <v>40724</v>
+        <v>40847</v>
       </c>
       <c r="B64" s="7">
         <v>3.25</v>
       </c>
       <c r="C64" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>UP</v>
+        <v>STAY</v>
       </c>
       <c r="D64" s="7">
         <v>6</v>
@@ -2004,10 +2007,10 @@
     </row>
     <row r="65" spans="1:6" ht="15" customHeight="1">
       <c r="A65" s="6">
-        <v>40694</v>
+        <v>40816</v>
       </c>
       <c r="B65" s="7">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="C65" s="7" t="str">
         <f t="shared" si="0"/>
@@ -2025,77 +2028,77 @@
     </row>
     <row r="66" spans="1:6" ht="15" customHeight="1">
       <c r="A66" s="6">
-        <v>40663</v>
+        <v>40786</v>
       </c>
       <c r="B66" s="7">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="C66" s="7" t="str">
-        <f t="shared" ref="C66:C129" si="1">IF(B66-B67=0,"STAY",IF(B66&gt;B67,"UP","DOWN"))</f>
+        <f t="shared" si="0"/>
         <v>STAY</v>
       </c>
       <c r="D66" s="7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E66" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="15" customHeight="1">
       <c r="A67" s="6">
-        <v>40633</v>
+        <v>40755</v>
       </c>
       <c r="B67" s="7">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="C67" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>UP</v>
+        <f t="shared" si="0"/>
+        <v>STAY</v>
       </c>
       <c r="D67" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E67" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="15" customHeight="1">
       <c r="A68" s="6">
-        <v>40602</v>
+        <v>40724</v>
       </c>
       <c r="B68" s="7">
-        <v>2.75</v>
+        <v>3.25</v>
       </c>
       <c r="C68" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>STAY</v>
+        <f t="shared" si="0"/>
+        <v>UP</v>
       </c>
       <c r="D68" s="7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E68" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="15" customHeight="1">
       <c r="A69" s="6">
-        <v>40574</v>
+        <v>40694</v>
       </c>
       <c r="B69" s="7">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="C69" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>UP</v>
+        <f t="shared" si="0"/>
+        <v>STAY</v>
       </c>
       <c r="D69" s="7">
         <v>4</v>
@@ -2104,82 +2107,82 @@
         <v>2</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="15" customHeight="1">
       <c r="A70" s="6">
-        <v>40543</v>
+        <v>40663</v>
       </c>
       <c r="B70" s="7">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="C70" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="C70:C133" si="1">IF(B70-B71=0,"STAY",IF(B70&gt;B71,"UP","DOWN"))</f>
         <v>STAY</v>
       </c>
       <c r="D70" s="7">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E70" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F70" s="7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="15" customHeight="1">
       <c r="A71" s="6">
-        <v>40512</v>
+        <v>40633</v>
       </c>
       <c r="B71" s="7">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="C71" s="7" t="str">
         <f t="shared" si="1"/>
         <v>UP</v>
       </c>
       <c r="D71" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E71" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F71" s="7" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="15" customHeight="1">
       <c r="A72" s="6">
-        <v>40482</v>
+        <v>40602</v>
       </c>
       <c r="B72" s="7">
-        <v>2.25</v>
+        <v>2.75</v>
       </c>
       <c r="C72" s="7" t="str">
         <f t="shared" si="1"/>
         <v>STAY</v>
       </c>
       <c r="D72" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E72" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F72" s="7" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="15" customHeight="1">
       <c r="A73" s="6">
-        <v>40451</v>
+        <v>40574</v>
       </c>
       <c r="B73" s="7">
-        <v>2.25</v>
+        <v>2.75</v>
       </c>
       <c r="C73" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>STAY</v>
+        <v>UP</v>
       </c>
       <c r="D73" s="7">
         <v>4</v>
@@ -2188,15 +2191,15 @@
         <v>2</v>
       </c>
       <c r="F73" s="7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="15" customHeight="1">
       <c r="A74" s="6">
-        <v>40421</v>
+        <v>40543</v>
       </c>
       <c r="B74" s="7">
-        <v>2.25</v>
+        <v>2.5</v>
       </c>
       <c r="C74" s="7" t="str">
         <f t="shared" si="1"/>
@@ -2214,73 +2217,73 @@
     </row>
     <row r="75" spans="1:6" ht="15" customHeight="1">
       <c r="A75" s="6">
-        <v>40390</v>
+        <v>40512</v>
       </c>
       <c r="B75" s="7">
-        <v>2.25</v>
+        <v>2.5</v>
       </c>
       <c r="C75" s="7" t="str">
         <f t="shared" si="1"/>
         <v>UP</v>
       </c>
       <c r="D75" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E75" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F75" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="15" customHeight="1">
       <c r="A76" s="6">
-        <v>40359</v>
+        <v>40482</v>
       </c>
       <c r="B76" s="7">
-        <v>2</v>
+        <v>2.25</v>
       </c>
       <c r="C76" s="7" t="str">
         <f t="shared" si="1"/>
         <v>STAY</v>
       </c>
       <c r="D76" s="7">
+        <v>5</v>
+      </c>
+      <c r="E76" s="7">
+        <v>1</v>
+      </c>
+      <c r="F76" s="7" t="s">
         <v>6</v>
-      </c>
-      <c r="E76" s="7">
-        <v>0</v>
-      </c>
-      <c r="F76" s="7" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="15" customHeight="1">
       <c r="A77" s="6">
-        <v>40329</v>
+        <v>40451</v>
       </c>
       <c r="B77" s="7">
-        <v>2</v>
+        <v>2.25</v>
       </c>
       <c r="C77" s="7" t="str">
         <f t="shared" si="1"/>
         <v>STAY</v>
       </c>
       <c r="D77" s="7">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E77" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F77" s="7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="15" customHeight="1">
       <c r="A78" s="6">
-        <v>40298</v>
+        <v>40421</v>
       </c>
       <c r="B78" s="7">
-        <v>2</v>
+        <v>2.25</v>
       </c>
       <c r="C78" s="7" t="str">
         <f t="shared" si="1"/>
@@ -2298,28 +2301,28 @@
     </row>
     <row r="79" spans="1:6" ht="15" customHeight="1">
       <c r="A79" s="6">
-        <v>40268</v>
+        <v>40390</v>
       </c>
       <c r="B79" s="7">
-        <v>2</v>
+        <v>2.25</v>
       </c>
       <c r="C79" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>STAY</v>
+        <v>UP</v>
       </c>
       <c r="D79" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E79" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F79" s="7" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="15" customHeight="1">
       <c r="A80" s="6">
-        <v>40237</v>
+        <v>40359</v>
       </c>
       <c r="B80" s="7">
         <v>2</v>
@@ -2335,12 +2338,12 @@
         <v>0</v>
       </c>
       <c r="F80" s="7" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="15" customHeight="1">
       <c r="A81" s="6">
-        <v>40209</v>
+        <v>40329</v>
       </c>
       <c r="B81" s="7">
         <v>2</v>
@@ -2361,7 +2364,7 @@
     </row>
     <row r="82" spans="1:6" ht="15" customHeight="1">
       <c r="A82" s="6">
-        <v>40178</v>
+        <v>40298</v>
       </c>
       <c r="B82" s="7">
         <v>2</v>
@@ -2370,13 +2373,19 @@
         <f t="shared" si="1"/>
         <v>STAY</v>
       </c>
-      <c r="D82" s="7"/>
-      <c r="E82" s="7"/>
-      <c r="F82" s="7"/>
+      <c r="D82" s="7">
+        <v>6</v>
+      </c>
+      <c r="E82" s="7">
+        <v>0</v>
+      </c>
+      <c r="F82" s="7" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="83" spans="1:6" ht="15" customHeight="1">
       <c r="A83" s="6">
-        <v>40147</v>
+        <v>40268</v>
       </c>
       <c r="B83" s="7">
         <v>2</v>
@@ -2385,13 +2394,19 @@
         <f t="shared" si="1"/>
         <v>STAY</v>
       </c>
-      <c r="D83" s="7"/>
-      <c r="E83" s="7"/>
-      <c r="F83" s="7"/>
+      <c r="D83" s="7">
+        <v>6</v>
+      </c>
+      <c r="E83" s="7">
+        <v>0</v>
+      </c>
+      <c r="F83" s="7" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="84" spans="1:6" ht="15" customHeight="1">
       <c r="A84" s="6">
-        <v>40117</v>
+        <v>40237</v>
       </c>
       <c r="B84" s="7">
         <v>2</v>
@@ -2400,13 +2415,19 @@
         <f t="shared" si="1"/>
         <v>STAY</v>
       </c>
-      <c r="D84" s="7"/>
-      <c r="E84" s="7"/>
-      <c r="F84" s="7"/>
+      <c r="D84" s="7">
+        <v>6</v>
+      </c>
+      <c r="E84" s="7">
+        <v>0</v>
+      </c>
+      <c r="F84" s="7" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="85" spans="1:6" ht="15" customHeight="1">
       <c r="A85" s="6">
-        <v>40086</v>
+        <v>40209</v>
       </c>
       <c r="B85" s="7">
         <v>2</v>
@@ -2415,13 +2436,19 @@
         <f t="shared" si="1"/>
         <v>STAY</v>
       </c>
-      <c r="D85" s="7"/>
-      <c r="E85" s="7"/>
-      <c r="F85" s="7"/>
+      <c r="D85" s="7">
+        <v>6</v>
+      </c>
+      <c r="E85" s="7">
+        <v>0</v>
+      </c>
+      <c r="F85" s="7" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="86" spans="1:6" ht="15" customHeight="1">
       <c r="A86" s="6">
-        <v>40056</v>
+        <v>40178</v>
       </c>
       <c r="B86" s="7">
         <v>2</v>
@@ -2436,7 +2463,7 @@
     </row>
     <row r="87" spans="1:6" ht="15" customHeight="1">
       <c r="A87" s="6">
-        <v>40025</v>
+        <v>40147</v>
       </c>
       <c r="B87" s="7">
         <v>2</v>
@@ -2451,7 +2478,7 @@
     </row>
     <row r="88" spans="1:6" ht="15" customHeight="1">
       <c r="A88" s="6">
-        <v>39994</v>
+        <v>40117</v>
       </c>
       <c r="B88" s="7">
         <v>2</v>
@@ -2466,7 +2493,7 @@
     </row>
     <row r="89" spans="1:6" ht="15" customHeight="1">
       <c r="A89" s="6">
-        <v>39964</v>
+        <v>40086</v>
       </c>
       <c r="B89" s="7">
         <v>2</v>
@@ -2481,7 +2508,7 @@
     </row>
     <row r="90" spans="1:6" ht="15" customHeight="1">
       <c r="A90" s="6">
-        <v>39933</v>
+        <v>40056</v>
       </c>
       <c r="B90" s="7">
         <v>2</v>
@@ -2496,7 +2523,7 @@
     </row>
     <row r="91" spans="1:6" ht="15" customHeight="1">
       <c r="A91" s="6">
-        <v>39903</v>
+        <v>40025</v>
       </c>
       <c r="B91" s="7">
         <v>2</v>
@@ -2511,14 +2538,14 @@
     </row>
     <row r="92" spans="1:6" ht="15" customHeight="1">
       <c r="A92" s="6">
-        <v>39872</v>
+        <v>39994</v>
       </c>
       <c r="B92" s="7">
         <v>2</v>
       </c>
       <c r="C92" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>DOWN</v>
+        <v>STAY</v>
       </c>
       <c r="D92" s="7"/>
       <c r="E92" s="7"/>
@@ -2526,14 +2553,14 @@
     </row>
     <row r="93" spans="1:6" ht="15" customHeight="1">
       <c r="A93" s="6">
-        <v>39844</v>
+        <v>39964</v>
       </c>
       <c r="B93" s="7">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="C93" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>DOWN</v>
+        <v>STAY</v>
       </c>
       <c r="D93" s="7"/>
       <c r="E93" s="7"/>
@@ -2541,14 +2568,14 @@
     </row>
     <row r="94" spans="1:6" ht="15" customHeight="1">
       <c r="A94" s="6">
-        <v>39813</v>
+        <v>39933</v>
       </c>
       <c r="B94" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C94" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>DOWN</v>
+        <v>STAY</v>
       </c>
       <c r="D94" s="7"/>
       <c r="E94" s="7"/>
@@ -2556,14 +2583,14 @@
     </row>
     <row r="95" spans="1:6" ht="15" customHeight="1">
       <c r="A95" s="6">
-        <v>39782</v>
+        <v>39903</v>
       </c>
       <c r="B95" s="7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C95" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>DOWN</v>
+        <v>STAY</v>
       </c>
       <c r="D95" s="7"/>
       <c r="E95" s="7"/>
@@ -2571,10 +2598,10 @@
     </row>
     <row r="96" spans="1:6" ht="15" customHeight="1">
       <c r="A96" s="6">
-        <v>39752</v>
+        <v>39872</v>
       </c>
       <c r="B96" s="7">
-        <v>4.25</v>
+        <v>2</v>
       </c>
       <c r="C96" s="7" t="str">
         <f t="shared" si="1"/>
@@ -2586,14 +2613,14 @@
     </row>
     <row r="97" spans="1:6" ht="15" customHeight="1">
       <c r="A97" s="6">
-        <v>39721</v>
+        <v>39844</v>
       </c>
       <c r="B97" s="7">
-        <v>5.25</v>
+        <v>2.5</v>
       </c>
       <c r="C97" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>STAY</v>
+        <v>DOWN</v>
       </c>
       <c r="D97" s="7"/>
       <c r="E97" s="7"/>
@@ -2601,14 +2628,14 @@
     </row>
     <row r="98" spans="1:6" ht="15" customHeight="1">
       <c r="A98" s="6">
-        <v>39691</v>
+        <v>39813</v>
       </c>
       <c r="B98" s="7">
-        <v>5.25</v>
+        <v>3</v>
       </c>
       <c r="C98" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>UP</v>
+        <v>DOWN</v>
       </c>
       <c r="D98" s="7"/>
       <c r="E98" s="7"/>
@@ -2616,14 +2643,14 @@
     </row>
     <row r="99" spans="1:6" ht="15" customHeight="1">
       <c r="A99" s="6">
-        <v>39660</v>
+        <v>39782</v>
       </c>
       <c r="B99" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C99" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>STAY</v>
+        <v>DOWN</v>
       </c>
       <c r="D99" s="7"/>
       <c r="E99" s="7"/>
@@ -2631,14 +2658,14 @@
     </row>
     <row r="100" spans="1:6" ht="15" customHeight="1">
       <c r="A100" s="6">
-        <v>39629</v>
+        <v>39752</v>
       </c>
       <c r="B100" s="7">
-        <v>5</v>
+        <v>4.25</v>
       </c>
       <c r="C100" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>STAY</v>
+        <v>DOWN</v>
       </c>
       <c r="D100" s="7"/>
       <c r="E100" s="7"/>
@@ -2646,10 +2673,10 @@
     </row>
     <row r="101" spans="1:6" ht="15" customHeight="1">
       <c r="A101" s="6">
-        <v>39599</v>
+        <v>39721</v>
       </c>
       <c r="B101" s="7">
-        <v>5</v>
+        <v>5.25</v>
       </c>
       <c r="C101" s="7" t="str">
         <f t="shared" si="1"/>
@@ -2661,14 +2688,14 @@
     </row>
     <row r="102" spans="1:6" ht="15" customHeight="1">
       <c r="A102" s="6">
-        <v>39568</v>
+        <v>39691</v>
       </c>
       <c r="B102" s="7">
-        <v>5</v>
+        <v>5.25</v>
       </c>
       <c r="C102" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>STAY</v>
+        <v>UP</v>
       </c>
       <c r="D102" s="7"/>
       <c r="E102" s="7"/>
@@ -2676,7 +2703,7 @@
     </row>
     <row r="103" spans="1:6" ht="15" customHeight="1">
       <c r="A103" s="6">
-        <v>39538</v>
+        <v>39660</v>
       </c>
       <c r="B103" s="7">
         <v>5</v>
@@ -2691,7 +2718,7 @@
     </row>
     <row r="104" spans="1:6" ht="15" customHeight="1">
       <c r="A104" s="6">
-        <v>39507</v>
+        <v>39629</v>
       </c>
       <c r="B104" s="7">
         <v>5</v>
@@ -2706,7 +2733,7 @@
     </row>
     <row r="105" spans="1:6" ht="15" customHeight="1">
       <c r="A105" s="6">
-        <v>39478</v>
+        <v>39599</v>
       </c>
       <c r="B105" s="7">
         <v>5</v>
@@ -2721,7 +2748,7 @@
     </row>
     <row r="106" spans="1:6" ht="15" customHeight="1">
       <c r="A106" s="6">
-        <v>39447</v>
+        <v>39568</v>
       </c>
       <c r="B106" s="7">
         <v>5</v>
@@ -2736,7 +2763,7 @@
     </row>
     <row r="107" spans="1:6" ht="15" customHeight="1">
       <c r="A107" s="6">
-        <v>39416</v>
+        <v>39538</v>
       </c>
       <c r="B107" s="7">
         <v>5</v>
@@ -2751,7 +2778,7 @@
     </row>
     <row r="108" spans="1:6" ht="15" customHeight="1">
       <c r="A108" s="6">
-        <v>39386</v>
+        <v>39507</v>
       </c>
       <c r="B108" s="7">
         <v>5</v>
@@ -2766,7 +2793,7 @@
     </row>
     <row r="109" spans="1:6" ht="15" customHeight="1">
       <c r="A109" s="6">
-        <v>39355</v>
+        <v>39478</v>
       </c>
       <c r="B109" s="7">
         <v>5</v>
@@ -2781,14 +2808,14 @@
     </row>
     <row r="110" spans="1:6" ht="15" customHeight="1">
       <c r="A110" s="6">
-        <v>39325</v>
+        <v>39447</v>
       </c>
       <c r="B110" s="7">
         <v>5</v>
       </c>
       <c r="C110" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>UP</v>
+        <v>STAY</v>
       </c>
       <c r="D110" s="7"/>
       <c r="E110" s="7"/>
@@ -2796,14 +2823,14 @@
     </row>
     <row r="111" spans="1:6" ht="15" customHeight="1">
       <c r="A111" s="6">
-        <v>39294</v>
+        <v>39416</v>
       </c>
       <c r="B111" s="7">
-        <v>4.75</v>
+        <v>5</v>
       </c>
       <c r="C111" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>UP</v>
+        <v>STAY</v>
       </c>
       <c r="D111" s="7"/>
       <c r="E111" s="7"/>
@@ -2811,10 +2838,10 @@
     </row>
     <row r="112" spans="1:6" ht="15" customHeight="1">
       <c r="A112" s="6">
-        <v>39263</v>
+        <v>39386</v>
       </c>
       <c r="B112" s="7">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="C112" s="7" t="str">
         <f t="shared" si="1"/>
@@ -2826,10 +2853,10 @@
     </row>
     <row r="113" spans="1:6" ht="15" customHeight="1">
       <c r="A113" s="6">
-        <v>39233</v>
+        <v>39355</v>
       </c>
       <c r="B113" s="7">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="C113" s="7" t="str">
         <f t="shared" si="1"/>
@@ -2841,14 +2868,14 @@
     </row>
     <row r="114" spans="1:6" ht="15" customHeight="1">
       <c r="A114" s="6">
-        <v>39202</v>
+        <v>39325</v>
       </c>
       <c r="B114" s="7">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="C114" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>STAY</v>
+        <v>UP</v>
       </c>
       <c r="D114" s="7"/>
       <c r="E114" s="7"/>
@@ -2856,14 +2883,14 @@
     </row>
     <row r="115" spans="1:6" ht="15" customHeight="1">
       <c r="A115" s="6">
-        <v>39172</v>
+        <v>39294</v>
       </c>
       <c r="B115" s="7">
-        <v>4.5</v>
+        <v>4.75</v>
       </c>
       <c r="C115" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>STAY</v>
+        <v>UP</v>
       </c>
       <c r="D115" s="7"/>
       <c r="E115" s="7"/>
@@ -2871,7 +2898,7 @@
     </row>
     <row r="116" spans="1:6" ht="15" customHeight="1">
       <c r="A116" s="6">
-        <v>39141</v>
+        <v>39263</v>
       </c>
       <c r="B116" s="7">
         <v>4.5</v>
@@ -2886,7 +2913,7 @@
     </row>
     <row r="117" spans="1:6" ht="15" customHeight="1">
       <c r="A117" s="6">
-        <v>39113</v>
+        <v>39233</v>
       </c>
       <c r="B117" s="7">
         <v>4.5</v>
@@ -2901,7 +2928,7 @@
     </row>
     <row r="118" spans="1:6" ht="15" customHeight="1">
       <c r="A118" s="6">
-        <v>39082</v>
+        <v>39202</v>
       </c>
       <c r="B118" s="7">
         <v>4.5</v>
@@ -2916,7 +2943,7 @@
     </row>
     <row r="119" spans="1:6" ht="15" customHeight="1">
       <c r="A119" s="6">
-        <v>39051</v>
+        <v>39172</v>
       </c>
       <c r="B119" s="7">
         <v>4.5</v>
@@ -2931,7 +2958,7 @@
     </row>
     <row r="120" spans="1:6" ht="15" customHeight="1">
       <c r="A120" s="6">
-        <v>39021</v>
+        <v>39141</v>
       </c>
       <c r="B120" s="7">
         <v>4.5</v>
@@ -2946,7 +2973,7 @@
     </row>
     <row r="121" spans="1:6" ht="15" customHeight="1">
       <c r="A121" s="6">
-        <v>38990</v>
+        <v>39113</v>
       </c>
       <c r="B121" s="7">
         <v>4.5</v>
@@ -2961,14 +2988,14 @@
     </row>
     <row r="122" spans="1:6" ht="15" customHeight="1">
       <c r="A122" s="6">
-        <v>38960</v>
+        <v>39082</v>
       </c>
       <c r="B122" s="7">
         <v>4.5</v>
       </c>
       <c r="C122" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>UP</v>
+        <v>STAY</v>
       </c>
       <c r="D122" s="7"/>
       <c r="E122" s="7"/>
@@ -2976,10 +3003,10 @@
     </row>
     <row r="123" spans="1:6" ht="15" customHeight="1">
       <c r="A123" s="6">
-        <v>38929</v>
+        <v>39051</v>
       </c>
       <c r="B123" s="7">
-        <v>4.25</v>
+        <v>4.5</v>
       </c>
       <c r="C123" s="7" t="str">
         <f t="shared" si="1"/>
@@ -2991,14 +3018,14 @@
     </row>
     <row r="124" spans="1:6" ht="15" customHeight="1">
       <c r="A124" s="6">
-        <v>38898</v>
+        <v>39021</v>
       </c>
       <c r="B124" s="7">
-        <v>4.25</v>
+        <v>4.5</v>
       </c>
       <c r="C124" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>UP</v>
+        <v>STAY</v>
       </c>
       <c r="D124" s="7"/>
       <c r="E124" s="7"/>
@@ -3006,10 +3033,10 @@
     </row>
     <row r="125" spans="1:6" ht="15" customHeight="1">
       <c r="A125" s="6">
-        <v>38868</v>
+        <v>38990</v>
       </c>
       <c r="B125" s="7">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="C125" s="7" t="str">
         <f t="shared" si="1"/>
@@ -3021,14 +3048,14 @@
     </row>
     <row r="126" spans="1:6" ht="15" customHeight="1">
       <c r="A126" s="6">
-        <v>38837</v>
+        <v>38960</v>
       </c>
       <c r="B126" s="7">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="C126" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>STAY</v>
+        <v>UP</v>
       </c>
       <c r="D126" s="7"/>
       <c r="E126" s="7"/>
@@ -3036,10 +3063,10 @@
     </row>
     <row r="127" spans="1:6" ht="15" customHeight="1">
       <c r="A127" s="6">
-        <v>38807</v>
+        <v>38929</v>
       </c>
       <c r="B127" s="7">
-        <v>4</v>
+        <v>4.25</v>
       </c>
       <c r="C127" s="7" t="str">
         <f t="shared" si="1"/>
@@ -3051,10 +3078,10 @@
     </row>
     <row r="128" spans="1:6" ht="15" customHeight="1">
       <c r="A128" s="6">
-        <v>38776</v>
+        <v>38898</v>
       </c>
       <c r="B128" s="7">
-        <v>4</v>
+        <v>4.25</v>
       </c>
       <c r="C128" s="7" t="str">
         <f t="shared" si="1"/>
@@ -3066,10 +3093,10 @@
     </row>
     <row r="129" spans="1:6" ht="15" customHeight="1">
       <c r="A129" s="6">
-        <v>38748</v>
+        <v>38868</v>
       </c>
       <c r="B129" s="7">
-        <v>3.75</v>
+        <v>4</v>
       </c>
       <c r="C129" s="7" t="str">
         <f t="shared" si="1"/>
@@ -3081,14 +3108,14 @@
     </row>
     <row r="130" spans="1:6" ht="15" customHeight="1">
       <c r="A130" s="6">
-        <v>38717</v>
+        <v>38837</v>
       </c>
       <c r="B130" s="7">
-        <v>3.75</v>
+        <v>4</v>
       </c>
       <c r="C130" s="7" t="str">
-        <f t="shared" ref="C130:C193" si="2">IF(B130-B131=0,"STAY",IF(B130&gt;B131,"UP","DOWN"))</f>
-        <v>UP</v>
+        <f t="shared" si="1"/>
+        <v>STAY</v>
       </c>
       <c r="D130" s="7"/>
       <c r="E130" s="7"/>
@@ -3096,13 +3123,13 @@
     </row>
     <row r="131" spans="1:6" ht="15" customHeight="1">
       <c r="A131" s="6">
-        <v>38686</v>
+        <v>38807</v>
       </c>
       <c r="B131" s="7">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="C131" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>STAY</v>
       </c>
       <c r="D131" s="7"/>
@@ -3111,13 +3138,13 @@
     </row>
     <row r="132" spans="1:6" ht="15" customHeight="1">
       <c r="A132" s="6">
-        <v>38656</v>
+        <v>38776</v>
       </c>
       <c r="B132" s="7">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="C132" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>UP</v>
       </c>
       <c r="D132" s="7"/>
@@ -3126,13 +3153,13 @@
     </row>
     <row r="133" spans="1:6" ht="15" customHeight="1">
       <c r="A133" s="6">
-        <v>38625</v>
+        <v>38748</v>
       </c>
       <c r="B133" s="7">
-        <v>3.25</v>
+        <v>3.75</v>
       </c>
       <c r="C133" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>STAY</v>
       </c>
       <c r="D133" s="7"/>
@@ -3141,14 +3168,14 @@
     </row>
     <row r="134" spans="1:6" ht="15" customHeight="1">
       <c r="A134" s="6">
-        <v>38595</v>
+        <v>38717</v>
       </c>
       <c r="B134" s="7">
-        <v>3.25</v>
+        <v>3.75</v>
       </c>
       <c r="C134" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>STAY</v>
+        <f t="shared" ref="C134:C197" si="2">IF(B134-B135=0,"STAY",IF(B134&gt;B135,"UP","DOWN"))</f>
+        <v>UP</v>
       </c>
       <c r="D134" s="7"/>
       <c r="E134" s="7"/>
@@ -3156,10 +3183,10 @@
     </row>
     <row r="135" spans="1:6" ht="15" customHeight="1">
       <c r="A135" s="6">
-        <v>38564</v>
+        <v>38686</v>
       </c>
       <c r="B135" s="7">
-        <v>3.25</v>
+        <v>3.5</v>
       </c>
       <c r="C135" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3171,14 +3198,14 @@
     </row>
     <row r="136" spans="1:6" ht="15" customHeight="1">
       <c r="A136" s="6">
-        <v>38533</v>
+        <v>38656</v>
       </c>
       <c r="B136" s="7">
-        <v>3.25</v>
+        <v>3.5</v>
       </c>
       <c r="C136" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>STAY</v>
+        <v>UP</v>
       </c>
       <c r="D136" s="7"/>
       <c r="E136" s="7"/>
@@ -3186,7 +3213,7 @@
     </row>
     <row r="137" spans="1:6" ht="15" customHeight="1">
       <c r="A137" s="6">
-        <v>38503</v>
+        <v>38625</v>
       </c>
       <c r="B137" s="7">
         <v>3.25</v>
@@ -3201,7 +3228,7 @@
     </row>
     <row r="138" spans="1:6" ht="15" customHeight="1">
       <c r="A138" s="6">
-        <v>38472</v>
+        <v>38595</v>
       </c>
       <c r="B138" s="7">
         <v>3.25</v>
@@ -3216,7 +3243,7 @@
     </row>
     <row r="139" spans="1:6" ht="15" customHeight="1">
       <c r="A139" s="6">
-        <v>38442</v>
+        <v>38564</v>
       </c>
       <c r="B139" s="7">
         <v>3.25</v>
@@ -3231,7 +3258,7 @@
     </row>
     <row r="140" spans="1:6" ht="15" customHeight="1">
       <c r="A140" s="6">
-        <v>38411</v>
+        <v>38533</v>
       </c>
       <c r="B140" s="7">
         <v>3.25</v>
@@ -3246,7 +3273,7 @@
     </row>
     <row r="141" spans="1:6" ht="15" customHeight="1">
       <c r="A141" s="6">
-        <v>38383</v>
+        <v>38503</v>
       </c>
       <c r="B141" s="7">
         <v>3.25</v>
@@ -3261,7 +3288,7 @@
     </row>
     <row r="142" spans="1:6" ht="15" customHeight="1">
       <c r="A142" s="6">
-        <v>38352</v>
+        <v>38472</v>
       </c>
       <c r="B142" s="7">
         <v>3.25</v>
@@ -3276,14 +3303,14 @@
     </row>
     <row r="143" spans="1:6" ht="15" customHeight="1">
       <c r="A143" s="6">
-        <v>38321</v>
+        <v>38442</v>
       </c>
       <c r="B143" s="7">
         <v>3.25</v>
       </c>
       <c r="C143" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>DOWN</v>
+        <v>STAY</v>
       </c>
       <c r="D143" s="7"/>
       <c r="E143" s="7"/>
@@ -3291,10 +3318,10 @@
     </row>
     <row r="144" spans="1:6" ht="15" customHeight="1">
       <c r="A144" s="6">
-        <v>38291</v>
+        <v>38411</v>
       </c>
       <c r="B144" s="7">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="C144" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3306,10 +3333,10 @@
     </row>
     <row r="145" spans="1:6" ht="15" customHeight="1">
       <c r="A145" s="6">
-        <v>38260</v>
+        <v>38383</v>
       </c>
       <c r="B145" s="7">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="C145" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3321,14 +3348,14 @@
     </row>
     <row r="146" spans="1:6" ht="15" customHeight="1">
       <c r="A146" s="6">
-        <v>38230</v>
+        <v>38352</v>
       </c>
       <c r="B146" s="7">
-        <v>3.5</v>
+        <v>3.25</v>
       </c>
       <c r="C146" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>DOWN</v>
+        <v>STAY</v>
       </c>
       <c r="D146" s="7"/>
       <c r="E146" s="7"/>
@@ -3336,14 +3363,14 @@
     </row>
     <row r="147" spans="1:6" ht="15" customHeight="1">
       <c r="A147" s="6">
-        <v>38199</v>
+        <v>38321</v>
       </c>
       <c r="B147" s="7">
-        <v>3.75</v>
+        <v>3.25</v>
       </c>
       <c r="C147" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>STAY</v>
+        <v>DOWN</v>
       </c>
       <c r="D147" s="7"/>
       <c r="E147" s="7"/>
@@ -3351,10 +3378,10 @@
     </row>
     <row r="148" spans="1:6" ht="15" customHeight="1">
       <c r="A148" s="6">
-        <v>38168</v>
+        <v>38291</v>
       </c>
       <c r="B148" s="7">
-        <v>3.75</v>
+        <v>3.5</v>
       </c>
       <c r="C148" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3366,10 +3393,10 @@
     </row>
     <row r="149" spans="1:6" ht="15" customHeight="1">
       <c r="A149" s="6">
-        <v>38138</v>
+        <v>38260</v>
       </c>
       <c r="B149" s="7">
-        <v>3.75</v>
+        <v>3.5</v>
       </c>
       <c r="C149" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3381,14 +3408,14 @@
     </row>
     <row r="150" spans="1:6" ht="15" customHeight="1">
       <c r="A150" s="6">
-        <v>38107</v>
+        <v>38230</v>
       </c>
       <c r="B150" s="7">
-        <v>3.75</v>
+        <v>3.5</v>
       </c>
       <c r="C150" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>STAY</v>
+        <v>DOWN</v>
       </c>
       <c r="D150" s="7"/>
       <c r="E150" s="7"/>
@@ -3396,7 +3423,7 @@
     </row>
     <row r="151" spans="1:6" ht="15" customHeight="1">
       <c r="A151" s="6">
-        <v>38077</v>
+        <v>38199</v>
       </c>
       <c r="B151" s="7">
         <v>3.75</v>
@@ -3411,7 +3438,7 @@
     </row>
     <row r="152" spans="1:6" ht="15" customHeight="1">
       <c r="A152" s="6">
-        <v>38046</v>
+        <v>38168</v>
       </c>
       <c r="B152" s="7">
         <v>3.75</v>
@@ -3426,7 +3453,7 @@
     </row>
     <row r="153" spans="1:6" ht="15" customHeight="1">
       <c r="A153" s="6">
-        <v>38017</v>
+        <v>38138</v>
       </c>
       <c r="B153" s="7">
         <v>3.75</v>
@@ -3441,7 +3468,7 @@
     </row>
     <row r="154" spans="1:6" ht="15" customHeight="1">
       <c r="A154" s="6">
-        <v>37986</v>
+        <v>38107</v>
       </c>
       <c r="B154" s="7">
         <v>3.75</v>
@@ -3456,7 +3483,7 @@
     </row>
     <row r="155" spans="1:6" ht="15" customHeight="1">
       <c r="A155" s="6">
-        <v>37955</v>
+        <v>38077</v>
       </c>
       <c r="B155" s="7">
         <v>3.75</v>
@@ -3471,7 +3498,7 @@
     </row>
     <row r="156" spans="1:6" ht="15" customHeight="1">
       <c r="A156" s="6">
-        <v>37925</v>
+        <v>38046</v>
       </c>
       <c r="B156" s="7">
         <v>3.75</v>
@@ -3486,7 +3513,7 @@
     </row>
     <row r="157" spans="1:6" ht="15" customHeight="1">
       <c r="A157" s="6">
-        <v>37894</v>
+        <v>38017</v>
       </c>
       <c r="B157" s="7">
         <v>3.75</v>
@@ -3501,7 +3528,7 @@
     </row>
     <row r="158" spans="1:6" ht="15" customHeight="1">
       <c r="A158" s="6">
-        <v>37864</v>
+        <v>37986</v>
       </c>
       <c r="B158" s="7">
         <v>3.75</v>
@@ -3516,14 +3543,14 @@
     </row>
     <row r="159" spans="1:6" ht="15" customHeight="1">
       <c r="A159" s="6">
-        <v>37833</v>
+        <v>37955</v>
       </c>
       <c r="B159" s="7">
         <v>3.75</v>
       </c>
       <c r="C159" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>DOWN</v>
+        <v>STAY</v>
       </c>
       <c r="D159" s="7"/>
       <c r="E159" s="7"/>
@@ -3531,10 +3558,10 @@
     </row>
     <row r="160" spans="1:6" ht="15" customHeight="1">
       <c r="A160" s="6">
-        <v>37802</v>
+        <v>37925</v>
       </c>
       <c r="B160" s="7">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="C160" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3546,14 +3573,14 @@
     </row>
     <row r="161" spans="1:6" ht="15" customHeight="1">
       <c r="A161" s="6">
-        <v>37772</v>
+        <v>37894</v>
       </c>
       <c r="B161" s="7">
-        <v>4</v>
+        <v>3.75</v>
       </c>
       <c r="C161" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>DOWN</v>
+        <v>STAY</v>
       </c>
       <c r="D161" s="7"/>
       <c r="E161" s="7"/>
@@ -3561,10 +3588,10 @@
     </row>
     <row r="162" spans="1:6" ht="15" customHeight="1">
       <c r="A162" s="6">
-        <v>37741</v>
+        <v>37864</v>
       </c>
       <c r="B162" s="7">
-        <v>4.25</v>
+        <v>3.75</v>
       </c>
       <c r="C162" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3576,14 +3603,14 @@
     </row>
     <row r="163" spans="1:6" ht="15" customHeight="1">
       <c r="A163" s="6">
-        <v>37711</v>
+        <v>37833</v>
       </c>
       <c r="B163" s="7">
-        <v>4.25</v>
+        <v>3.75</v>
       </c>
       <c r="C163" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>STAY</v>
+        <v>DOWN</v>
       </c>
       <c r="D163" s="7"/>
       <c r="E163" s="7"/>
@@ -3591,10 +3618,10 @@
     </row>
     <row r="164" spans="1:6" ht="15" customHeight="1">
       <c r="A164" s="6">
-        <v>37680</v>
+        <v>37802</v>
       </c>
       <c r="B164" s="7">
-        <v>4.25</v>
+        <v>4</v>
       </c>
       <c r="C164" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3606,14 +3633,14 @@
     </row>
     <row r="165" spans="1:6" ht="15" customHeight="1">
       <c r="A165" s="6">
-        <v>37652</v>
+        <v>37772</v>
       </c>
       <c r="B165" s="7">
-        <v>4.25</v>
+        <v>4</v>
       </c>
       <c r="C165" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>STAY</v>
+        <v>DOWN</v>
       </c>
       <c r="D165" s="7"/>
       <c r="E165" s="7"/>
@@ -3621,7 +3648,7 @@
     </row>
     <row r="166" spans="1:6" ht="15" customHeight="1">
       <c r="A166" s="6">
-        <v>37621</v>
+        <v>37741</v>
       </c>
       <c r="B166" s="7">
         <v>4.25</v>
@@ -3636,7 +3663,7 @@
     </row>
     <row r="167" spans="1:6" ht="15" customHeight="1">
       <c r="A167" s="6">
-        <v>37590</v>
+        <v>37711</v>
       </c>
       <c r="B167" s="7">
         <v>4.25</v>
@@ -3651,7 +3678,7 @@
     </row>
     <row r="168" spans="1:6" ht="15" customHeight="1">
       <c r="A168" s="6">
-        <v>37560</v>
+        <v>37680</v>
       </c>
       <c r="B168" s="7">
         <v>4.25</v>
@@ -3666,7 +3693,7 @@
     </row>
     <row r="169" spans="1:6" ht="15" customHeight="1">
       <c r="A169" s="6">
-        <v>37529</v>
+        <v>37652</v>
       </c>
       <c r="B169" s="7">
         <v>4.25</v>
@@ -3681,7 +3708,7 @@
     </row>
     <row r="170" spans="1:6" ht="15" customHeight="1">
       <c r="A170" s="6">
-        <v>37499</v>
+        <v>37621</v>
       </c>
       <c r="B170" s="7">
         <v>4.25</v>
@@ -3696,7 +3723,7 @@
     </row>
     <row r="171" spans="1:6" ht="15" customHeight="1">
       <c r="A171" s="6">
-        <v>37468</v>
+        <v>37590</v>
       </c>
       <c r="B171" s="7">
         <v>4.25</v>
@@ -3711,7 +3738,7 @@
     </row>
     <row r="172" spans="1:6" ht="15" customHeight="1">
       <c r="A172" s="6">
-        <v>37437</v>
+        <v>37560</v>
       </c>
       <c r="B172" s="7">
         <v>4.25</v>
@@ -3726,14 +3753,14 @@
     </row>
     <row r="173" spans="1:6" ht="15" customHeight="1">
       <c r="A173" s="6">
-        <v>37407</v>
+        <v>37529</v>
       </c>
       <c r="B173" s="7">
         <v>4.25</v>
       </c>
       <c r="C173" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>UP</v>
+        <v>STAY</v>
       </c>
       <c r="D173" s="7"/>
       <c r="E173" s="7"/>
@@ -3741,10 +3768,10 @@
     </row>
     <row r="174" spans="1:6" ht="15" customHeight="1">
       <c r="A174" s="6">
-        <v>37376</v>
+        <v>37499</v>
       </c>
       <c r="B174" s="7">
-        <v>4</v>
+        <v>4.25</v>
       </c>
       <c r="C174" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3756,10 +3783,10 @@
     </row>
     <row r="175" spans="1:6" ht="15" customHeight="1">
       <c r="A175" s="6">
-        <v>37346</v>
+        <v>37468</v>
       </c>
       <c r="B175" s="7">
-        <v>4</v>
+        <v>4.25</v>
       </c>
       <c r="C175" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3771,10 +3798,10 @@
     </row>
     <row r="176" spans="1:6" ht="15" customHeight="1">
       <c r="A176" s="6">
-        <v>37315</v>
+        <v>37437</v>
       </c>
       <c r="B176" s="7">
-        <v>4</v>
+        <v>4.25</v>
       </c>
       <c r="C176" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3786,14 +3813,14 @@
     </row>
     <row r="177" spans="1:6" ht="15" customHeight="1">
       <c r="A177" s="6">
-        <v>37287</v>
+        <v>37407</v>
       </c>
       <c r="B177" s="7">
-        <v>4</v>
+        <v>4.25</v>
       </c>
       <c r="C177" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>STAY</v>
+        <v>UP</v>
       </c>
       <c r="D177" s="7"/>
       <c r="E177" s="7"/>
@@ -3801,7 +3828,7 @@
     </row>
     <row r="178" spans="1:6" ht="15" customHeight="1">
       <c r="A178" s="6">
-        <v>37256</v>
+        <v>37376</v>
       </c>
       <c r="B178" s="7">
         <v>4</v>
@@ -3816,7 +3843,7 @@
     </row>
     <row r="179" spans="1:6" ht="15" customHeight="1">
       <c r="A179" s="6">
-        <v>37225</v>
+        <v>37346</v>
       </c>
       <c r="B179" s="7">
         <v>4</v>
@@ -3831,7 +3858,7 @@
     </row>
     <row r="180" spans="1:6" ht="15" customHeight="1">
       <c r="A180" s="6">
-        <v>37195</v>
+        <v>37315</v>
       </c>
       <c r="B180" s="7">
         <v>4</v>
@@ -3846,14 +3873,14 @@
     </row>
     <row r="181" spans="1:6" ht="15" customHeight="1">
       <c r="A181" s="6">
-        <v>37164</v>
+        <v>37287</v>
       </c>
       <c r="B181" s="7">
         <v>4</v>
       </c>
       <c r="C181" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>DOWN</v>
+        <v>STAY</v>
       </c>
       <c r="D181" s="7"/>
       <c r="E181" s="7"/>
@@ -3861,14 +3888,14 @@
     </row>
     <row r="182" spans="1:6" ht="15" customHeight="1">
       <c r="A182" s="6">
-        <v>37134</v>
+        <v>37256</v>
       </c>
       <c r="B182" s="7">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="C182" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>DOWN</v>
+        <v>STAY</v>
       </c>
       <c r="D182" s="7"/>
       <c r="E182" s="7"/>
@@ -3876,14 +3903,14 @@
     </row>
     <row r="183" spans="1:6" ht="15" customHeight="1">
       <c r="A183" s="6">
-        <v>37103</v>
+        <v>37225</v>
       </c>
       <c r="B183" s="7">
-        <v>4.75</v>
+        <v>4</v>
       </c>
       <c r="C183" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>DOWN</v>
+        <v>STAY</v>
       </c>
       <c r="D183" s="7"/>
       <c r="E183" s="7"/>
@@ -3891,10 +3918,10 @@
     </row>
     <row r="184" spans="1:6" ht="15" customHeight="1">
       <c r="A184" s="6">
-        <v>37072</v>
+        <v>37195</v>
       </c>
       <c r="B184" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C184" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3906,14 +3933,14 @@
     </row>
     <row r="185" spans="1:6" ht="15" customHeight="1">
       <c r="A185" s="6">
-        <v>37042</v>
+        <v>37164</v>
       </c>
       <c r="B185" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C185" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>STAY</v>
+        <v>DOWN</v>
       </c>
       <c r="D185" s="7"/>
       <c r="E185" s="7"/>
@@ -3921,14 +3948,14 @@
     </row>
     <row r="186" spans="1:6" ht="15" customHeight="1">
       <c r="A186" s="6">
-        <v>37011</v>
+        <v>37134</v>
       </c>
       <c r="B186" s="7">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="C186" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>STAY</v>
+        <v>DOWN</v>
       </c>
       <c r="D186" s="7"/>
       <c r="E186" s="7"/>
@@ -3936,14 +3963,14 @@
     </row>
     <row r="187" spans="1:6" ht="15" customHeight="1">
       <c r="A187" s="6">
-        <v>36981</v>
+        <v>37103</v>
       </c>
       <c r="B187" s="7">
-        <v>5</v>
+        <v>4.75</v>
       </c>
       <c r="C187" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>STAY</v>
+        <v>DOWN</v>
       </c>
       <c r="D187" s="7"/>
       <c r="E187" s="7"/>
@@ -3951,14 +3978,14 @@
     </row>
     <row r="188" spans="1:6" ht="15" customHeight="1">
       <c r="A188" s="6">
-        <v>36950</v>
+        <v>37072</v>
       </c>
       <c r="B188" s="7">
         <v>5</v>
       </c>
       <c r="C188" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>DOWN</v>
+        <v>STAY</v>
       </c>
       <c r="D188" s="7"/>
       <c r="E188" s="7"/>
@@ -3966,10 +3993,10 @@
     </row>
     <row r="189" spans="1:6" ht="15" customHeight="1">
       <c r="A189" s="6">
-        <v>36922</v>
+        <v>37042</v>
       </c>
       <c r="B189" s="7">
-        <v>5.25</v>
+        <v>5</v>
       </c>
       <c r="C189" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3981,10 +4008,10 @@
     </row>
     <row r="190" spans="1:6" ht="15" customHeight="1">
       <c r="A190" s="6">
-        <v>36891</v>
+        <v>37011</v>
       </c>
       <c r="B190" s="7">
-        <v>5.25</v>
+        <v>5</v>
       </c>
       <c r="C190" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3996,10 +4023,10 @@
     </row>
     <row r="191" spans="1:6" ht="15" customHeight="1">
       <c r="A191" s="6">
-        <v>36860</v>
+        <v>36981</v>
       </c>
       <c r="B191" s="7">
-        <v>5.25</v>
+        <v>5</v>
       </c>
       <c r="C191" s="7" t="str">
         <f t="shared" si="2"/>
@@ -4011,14 +4038,14 @@
     </row>
     <row r="192" spans="1:6" ht="15" customHeight="1">
       <c r="A192" s="6">
-        <v>36830</v>
+        <v>36950</v>
       </c>
       <c r="B192" s="7">
-        <v>5.25</v>
+        <v>5</v>
       </c>
       <c r="C192" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>UP</v>
+        <v>DOWN</v>
       </c>
       <c r="D192" s="7"/>
       <c r="E192" s="7"/>
@@ -4026,10 +4053,10 @@
     </row>
     <row r="193" spans="1:6" ht="15" customHeight="1">
       <c r="A193" s="6">
-        <v>36799</v>
+        <v>36922</v>
       </c>
       <c r="B193" s="7">
-        <v>5</v>
+        <v>5.25</v>
       </c>
       <c r="C193" s="7" t="str">
         <f t="shared" si="2"/>
@@ -4041,13 +4068,13 @@
     </row>
     <row r="194" spans="1:6" ht="15" customHeight="1">
       <c r="A194" s="6">
-        <v>36769</v>
+        <v>36891</v>
       </c>
       <c r="B194" s="7">
-        <v>5</v>
+        <v>5.25</v>
       </c>
       <c r="C194" s="7" t="str">
-        <f t="shared" ref="C194:C209" si="3">IF(B194-B195=0,"STAY",IF(B194&gt;B195,"UP","DOWN"))</f>
+        <f t="shared" si="2"/>
         <v>STAY</v>
       </c>
       <c r="D194" s="7"/>
@@ -4056,13 +4083,13 @@
     </row>
     <row r="195" spans="1:6" ht="15" customHeight="1">
       <c r="A195" s="6">
-        <v>36738</v>
+        <v>36860</v>
       </c>
       <c r="B195" s="7">
-        <v>5</v>
+        <v>5.25</v>
       </c>
       <c r="C195" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>STAY</v>
       </c>
       <c r="D195" s="7"/>
@@ -4071,14 +4098,14 @@
     </row>
     <row r="196" spans="1:6" ht="15" customHeight="1">
       <c r="A196" s="6">
-        <v>36707</v>
+        <v>36830</v>
       </c>
       <c r="B196" s="7">
-        <v>5</v>
+        <v>5.25</v>
       </c>
       <c r="C196" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>STAY</v>
+        <f t="shared" si="2"/>
+        <v>UP</v>
       </c>
       <c r="D196" s="7"/>
       <c r="E196" s="7"/>
@@ -4086,13 +4113,13 @@
     </row>
     <row r="197" spans="1:6" ht="15" customHeight="1">
       <c r="A197" s="6">
-        <v>36677</v>
+        <v>36799</v>
       </c>
       <c r="B197" s="7">
         <v>5</v>
       </c>
       <c r="C197" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>STAY</v>
       </c>
       <c r="D197" s="7"/>
@@ -4101,13 +4128,13 @@
     </row>
     <row r="198" spans="1:6" ht="15" customHeight="1">
       <c r="A198" s="6">
-        <v>36646</v>
+        <v>36769</v>
       </c>
       <c r="B198" s="7">
         <v>5</v>
       </c>
       <c r="C198" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="C198:C213" si="3">IF(B198-B199=0,"STAY",IF(B198&gt;B199,"UP","DOWN"))</f>
         <v>STAY</v>
       </c>
       <c r="D198" s="7"/>
@@ -4116,7 +4143,7 @@
     </row>
     <row r="199" spans="1:6" ht="15" customHeight="1">
       <c r="A199" s="6">
-        <v>36616</v>
+        <v>36738</v>
       </c>
       <c r="B199" s="7">
         <v>5</v>
@@ -4131,14 +4158,14 @@
     </row>
     <row r="200" spans="1:6" ht="15" customHeight="1">
       <c r="A200" s="6">
-        <v>36585</v>
+        <v>36707</v>
       </c>
       <c r="B200" s="7">
         <v>5</v>
       </c>
       <c r="C200" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>UP</v>
+        <v>STAY</v>
       </c>
       <c r="D200" s="7"/>
       <c r="E200" s="7"/>
@@ -4146,10 +4173,10 @@
     </row>
     <row r="201" spans="1:6" ht="15" customHeight="1">
       <c r="A201" s="6">
-        <v>36556</v>
+        <v>36677</v>
       </c>
       <c r="B201" s="7">
-        <v>4.75</v>
+        <v>5</v>
       </c>
       <c r="C201" s="7" t="str">
         <f t="shared" si="3"/>
@@ -4161,10 +4188,10 @@
     </row>
     <row r="202" spans="1:6" ht="15" customHeight="1">
       <c r="A202" s="6">
-        <v>36525</v>
+        <v>36646</v>
       </c>
       <c r="B202" s="7">
-        <v>4.75</v>
+        <v>5</v>
       </c>
       <c r="C202" s="7" t="str">
         <f t="shared" si="3"/>
@@ -4176,10 +4203,10 @@
     </row>
     <row r="203" spans="1:6" ht="15" customHeight="1">
       <c r="A203" s="6">
-        <v>36494</v>
+        <v>36616</v>
       </c>
       <c r="B203" s="7">
-        <v>4.75</v>
+        <v>5</v>
       </c>
       <c r="C203" s="7" t="str">
         <f t="shared" si="3"/>
@@ -4191,14 +4218,14 @@
     </row>
     <row r="204" spans="1:6" ht="15" customHeight="1">
       <c r="A204" s="6">
-        <v>36464</v>
+        <v>36585</v>
       </c>
       <c r="B204" s="7">
-        <v>4.75</v>
+        <v>5</v>
       </c>
       <c r="C204" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>STAY</v>
+        <v>UP</v>
       </c>
       <c r="D204" s="7"/>
       <c r="E204" s="7"/>
@@ -4206,7 +4233,7 @@
     </row>
     <row r="205" spans="1:6" ht="15" customHeight="1">
       <c r="A205" s="6">
-        <v>36433</v>
+        <v>36556</v>
       </c>
       <c r="B205" s="7">
         <v>4.75</v>
@@ -4221,7 +4248,7 @@
     </row>
     <row r="206" spans="1:6" ht="15" customHeight="1">
       <c r="A206" s="6">
-        <v>36403</v>
+        <v>36525</v>
       </c>
       <c r="B206" s="7">
         <v>4.75</v>
@@ -4236,7 +4263,7 @@
     </row>
     <row r="207" spans="1:6" ht="15" customHeight="1">
       <c r="A207" s="6">
-        <v>36372</v>
+        <v>36494</v>
       </c>
       <c r="B207" s="7">
         <v>4.75</v>
@@ -4251,7 +4278,7 @@
     </row>
     <row r="208" spans="1:6" ht="15" customHeight="1">
       <c r="A208" s="6">
-        <v>36341</v>
+        <v>36464</v>
       </c>
       <c r="B208" s="7">
         <v>4.75</v>
@@ -4266,77 +4293,137 @@
     </row>
     <row r="209" spans="1:6" ht="15" customHeight="1">
       <c r="A209" s="6">
-        <v>36311</v>
+        <v>36433</v>
       </c>
       <c r="B209" s="7">
         <v>4.75</v>
       </c>
       <c r="C209" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>UP</v>
+        <v>STAY</v>
       </c>
       <c r="D209" s="7"/>
       <c r="E209" s="7"/>
       <c r="F209" s="7"/>
     </row>
     <row r="210" spans="1:6" ht="15" customHeight="1">
-      <c r="A210" s="7"/>
-      <c r="B210" s="7"/>
-      <c r="C210" s="7"/>
-      <c r="D210" s="7" t="s">
+      <c r="A210" s="6">
+        <v>36403</v>
+      </c>
+      <c r="B210" s="7">
+        <v>4.75</v>
+      </c>
+      <c r="C210" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>STAY</v>
+      </c>
+      <c r="D210" s="7"/>
+      <c r="E210" s="7"/>
+      <c r="F210" s="7"/>
+    </row>
+    <row r="211" spans="1:6" ht="15" customHeight="1">
+      <c r="A211" s="6">
+        <v>36372</v>
+      </c>
+      <c r="B211" s="7">
+        <v>4.75</v>
+      </c>
+      <c r="C211" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>STAY</v>
+      </c>
+      <c r="D211" s="7"/>
+      <c r="E211" s="7"/>
+      <c r="F211" s="7"/>
+    </row>
+    <row r="212" spans="1:6" ht="15" customHeight="1">
+      <c r="A212" s="6">
+        <v>36341</v>
+      </c>
+      <c r="B212" s="7">
+        <v>4.75</v>
+      </c>
+      <c r="C212" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>STAY</v>
+      </c>
+      <c r="D212" s="7"/>
+      <c r="E212" s="7"/>
+      <c r="F212" s="7"/>
+    </row>
+    <row r="213" spans="1:6" ht="15" customHeight="1">
+      <c r="A213" s="6">
+        <v>36311</v>
+      </c>
+      <c r="B213" s="7">
+        <v>4.75</v>
+      </c>
+      <c r="C213" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>UP</v>
+      </c>
+      <c r="D213" s="7"/>
+      <c r="E213" s="7"/>
+      <c r="F213" s="7"/>
+    </row>
+    <row r="214" spans="1:6" ht="15" customHeight="1">
+      <c r="A214" s="7"/>
+      <c r="B214" s="7"/>
+      <c r="C214" s="7"/>
+      <c r="D214" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E210" s="7">
-        <f>COUNTIF($C$2:$C$209,"UP")</f>
+      <c r="E214" s="7">
+        <f>COUNTIF($C$6:$C$213,"UP")</f>
         <v>17</v>
       </c>
-      <c r="F210" s="8">
-        <f>E210/$E$213</f>
+      <c r="F214" s="8">
+        <f>E214/$E$217</f>
         <v>8.1730769230769232E-2</v>
       </c>
     </row>
-    <row r="211" spans="1:6" ht="15" customHeight="1">
-      <c r="A211" s="7"/>
-      <c r="B211" s="7"/>
-      <c r="C211" s="7"/>
-      <c r="D211" s="7" t="s">
+    <row r="215" spans="1:6" ht="15" customHeight="1">
+      <c r="A215" s="7"/>
+      <c r="B215" s="7"/>
+      <c r="C215" s="7"/>
+      <c r="D215" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E211" s="7">
-        <f>COUNTIF($C$2:$C$209,"DOWN")</f>
+      <c r="E215" s="7">
+        <f>COUNTIF($C$6:$C$213,"DOWN")</f>
         <v>21</v>
       </c>
-      <c r="F211" s="8">
-        <f t="shared" ref="F211:F212" si="4">E211/$E$213</f>
+      <c r="F215" s="8">
+        <f t="shared" ref="F215:F216" si="4">E215/$E$217</f>
         <v>0.10096153846153846</v>
       </c>
     </row>
-    <row r="212" spans="1:6" ht="15" customHeight="1">
-      <c r="A212" s="7"/>
-      <c r="B212" s="7"/>
-      <c r="C212" s="7"/>
-      <c r="D212" s="7" t="s">
+    <row r="216" spans="1:6" ht="15" customHeight="1">
+      <c r="A216" s="7"/>
+      <c r="B216" s="7"/>
+      <c r="C216" s="7"/>
+      <c r="D216" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E212" s="7">
-        <f>COUNTIF($C$2:$C$209,"STAY")</f>
+      <c r="E216" s="7">
+        <f>COUNTIF($C$6:$C$213,"STAY")</f>
         <v>170</v>
       </c>
-      <c r="F212" s="8">
+      <c r="F216" s="8">
         <f t="shared" si="4"/>
         <v>0.81730769230769229</v>
       </c>
     </row>
-    <row r="213" spans="1:6" ht="15" customHeight="1">
-      <c r="A213" s="7"/>
-      <c r="B213" s="7"/>
-      <c r="C213" s="7"/>
-      <c r="D213" s="7"/>
-      <c r="E213" s="7">
-        <f>SUM(E210:E212)</f>
+    <row r="217" spans="1:6" ht="15" customHeight="1">
+      <c r="A217" s="7"/>
+      <c r="B217" s="7"/>
+      <c r="C217" s="7"/>
+      <c r="D217" s="7"/>
+      <c r="E217" s="7">
+        <f>SUM(E214:E216)</f>
         <v>208</v>
       </c>
-      <c r="F213" s="7"/>
+      <c r="F217" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>